<commit_message>
18th August 2022 - Session
</commit_message>
<xml_diff>
--- a/examhub.xlsx
+++ b/examhub.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ns_neutron\neutron_sql_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\ns_neutron\api_examhub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC35BDE-1E80-4A37-8424-22F30B60FFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516378BC-5A72-42A8-A08D-01641CA6A5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{836053F9-EBCC-45F2-8D08-2C10A12D37D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{836053F9-EBCC-45F2-8D08-2C10A12D37D6}"/>
   </bookViews>
   <sheets>
     <sheet name="DB Table" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="242">
   <si>
     <t>Types of login - candidate &lt; teachers &lt; admin</t>
   </si>
@@ -654,6 +654,117 @@
   </si>
   <si>
     <t>http://localhost:4000/questions/getquestionbysubject/?subject=1&amp;count=2</t>
+  </si>
+  <si>
+    <t>exam_id</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>total_questions</t>
+  </si>
+  <si>
+    <t>subject1</t>
+  </si>
+  <si>
+    <t>numqs1</t>
+  </si>
+  <si>
+    <t>subject2</t>
+  </si>
+  <si>
+    <t>numqs2</t>
+  </si>
+  <si>
+    <t>subject3</t>
+  </si>
+  <si>
+    <t>numqs3</t>
+  </si>
+  <si>
+    <t>subject4</t>
+  </si>
+  <si>
+    <t>numqs4</t>
+  </si>
+  <si>
+    <t>subject5</t>
+  </si>
+  <si>
+    <t>numqs5</t>
+  </si>
+  <si>
+    <t>[{'1', 10}, {'4', 15}, {'5', 20}]</t>
+  </si>
+  <si>
+    <t>qs - [], multiple rows</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>exam_log_id</t>
+  </si>
+  <si>
+    <t>exam_name</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY, AUTO INCREMENT, INT</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>INT - NOT NULL</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>negativemarking</t>
+  </si>
+  <si>
+    <t>exams</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/exams/createexam</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/exams/fetchallexams</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/exams/updateexam</t>
+  </si>
+  <si>
+    <t>http://localhost:4000/exams/removeexam/exam_id</t>
+  </si>
+  <si>
+    <t>Body - exam_name, subject_id, duration, total_questions</t>
+  </si>
+  <si>
+    <t>Body - exam_id, exam_name, subject_id, duration, total_questions</t>
+  </si>
+  <si>
+    <t>create exam</t>
+  </si>
+  <si>
+    <t>update exam</t>
+  </si>
+  <si>
+    <t>delete exam</t>
+  </si>
+  <si>
+    <t>get list of all exams</t>
   </si>
 </sst>
 </file>
@@ -770,7 +881,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -815,6 +926,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1130,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598E409D-B184-44C1-9772-DD09FE403E30}">
-  <dimension ref="C3:R23"/>
+  <dimension ref="C2:S37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1150,14 +1263,26 @@
     <col min="10" max="10" width="3.109375" style="23" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
     <col min="12" max="12" width="3.109375" style="23" customWidth="1"/>
-    <col min="14" max="14" width="18.5546875" customWidth="1"/>
-    <col min="15" max="15" width="3.109375" style="23" customWidth="1"/>
-    <col min="16" max="16" width="14.77734375" customWidth="1"/>
-    <col min="17" max="17" width="17.21875" customWidth="1"/>
-    <col min="18" max="18" width="3.109375" style="23" customWidth="1"/>
+    <col min="14" max="14" width="36.109375" customWidth="1"/>
+    <col min="15" max="15" width="18.5546875" customWidth="1"/>
+    <col min="16" max="16" width="3.109375" style="23" customWidth="1"/>
+    <col min="17" max="17" width="14.77734375" customWidth="1"/>
+    <col min="18" max="18" width="17.21875" customWidth="1"/>
+    <col min="19" max="19" width="3.109375" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>222</v>
+      </c>
+      <c r="K2" t="s">
+        <v>222</v>
+      </c>
+      <c r="O2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1181,19 +1306,20 @@
       <c r="M3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="1"/>
+      <c r="O3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="22"/>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="22"/>
+      <c r="Q3" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="R3" s="22"/>
-    </row>
-    <row r="4" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="S3" s="22"/>
+    </row>
+    <row r="4" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C4" s="8" t="s">
         <v>20</v>
       </c>
@@ -1212,8 +1338,20 @@
       <c r="K4" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="M4" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="N4" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="O4" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
@@ -1232,8 +1370,17 @@
       <c r="K5" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="M5" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="O5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C6" s="9" t="s">
         <v>22</v>
       </c>
@@ -1249,8 +1396,14 @@
       <c r="K6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="M6" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="N6" s="24" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1263,8 +1416,14 @@
       <c r="G7" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="M7" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="N7" s="24" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>24</v>
       </c>
@@ -1277,8 +1436,14 @@
       <c r="G8" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="M8" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="N8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>26</v>
       </c>
@@ -1291,8 +1456,14 @@
       <c r="G9" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="M9" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="N9" s="24" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C10" s="11" t="s">
         <v>32</v>
       </c>
@@ -1305,8 +1476,14 @@
       <c r="G10" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="M10" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="N10" s="24" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>39</v>
       </c>
@@ -1322,8 +1499,11 @@
       <c r="I11" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="M11" s="24" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="3:19" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>35</v>
       </c>
@@ -1337,7 +1517,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
       <c r="D13" t="s">
         <v>36</v>
@@ -1352,7 +1532,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
       <c r="D14" t="s">
         <v>37</v>
@@ -1367,7 +1547,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:19" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>38</v>
       </c>
@@ -1381,7 +1561,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:19" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>72</v>
       </c>
@@ -1389,7 +1569,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>73</v>
       </c>
@@ -1397,14 +1577,72 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C23" s="9"/>
       <c r="D23" s="6"/>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="M25" t="s">
+        <v>41</v>
+      </c>
+      <c r="O25" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="M28" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="M29" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="M30" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="M31" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="M32" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M33" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M36" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M37" t="s">
+        <v>219</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1416,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EF03A8-C01B-4EC5-9622-342E1F504EDA}">
   <dimension ref="C3:O47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2937,14 +3175,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBCD982-A1F7-4F12-9554-A4111D34D39C}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
     <col min="7" max="7" width="67.21875" customWidth="1"/>
     <col min="8" max="8" width="43.77734375" customWidth="1"/>
@@ -3152,7 +3391,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="4:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D17" s="4">
         <v>12</v>
       </c>
@@ -3166,7 +3405,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="18" spans="4:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D18" s="4">
         <v>13</v>
       </c>
@@ -3178,6 +3417,74 @@
       </c>
       <c r="G18" s="5" t="s">
         <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D22" s="4">
+        <v>14</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="4">
+        <v>15</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="4">
+        <v>16</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="4">
+        <v>17</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3194,8 +3501,12 @@
     <hyperlink ref="G16" r:id="rId10" xr:uid="{35BFFB03-C142-47BD-897D-7983C61F6FCE}"/>
     <hyperlink ref="G17" r:id="rId11" xr:uid="{A6AD5FE8-090D-469D-B831-49F3D53948E1}"/>
     <hyperlink ref="G18" r:id="rId12" xr:uid="{DB769738-BE36-4429-96A8-10652DC6D6B1}"/>
+    <hyperlink ref="G22" r:id="rId13" xr:uid="{82F0BE54-5A8E-414D-AB4D-85BDCB6E4893}"/>
+    <hyperlink ref="G23" r:id="rId14" xr:uid="{2D172DE5-206B-4CED-979C-A667C296DCE9}"/>
+    <hyperlink ref="G24" r:id="rId15" xr:uid="{4FC2C38E-8CBD-4AE6-A5D4-B82228F0B505}"/>
+    <hyperlink ref="G25" r:id="rId16" xr:uid="{34CA76FC-0CAB-44CD-90D7-70F615CDA84E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>